<commit_message>
Correção de Data no Termo
</commit_message>
<xml_diff>
--- a/CARGOS_FILTRADOS.xlsx
+++ b/CARGOS_FILTRADOS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,36 +497,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>COLABORADOR 4</t>
+          <t>COLABORADOR 1</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>30628</v>
+        <v>29243</v>
       </c>
       <c r="C2" t="n">
-        <v>56345128997</v>
+        <v>48194946080</v>
       </c>
       <c r="D2" t="n">
-        <v>6718754</v>
+        <v>8630400</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ORG2</t>
+          <t>ORG1</t>
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>24422</v>
+        <v>32403</v>
       </c>
       <c r="G2" t="n">
-        <v>16468397872</v>
+        <v>33493360793</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>colaborador4@outlook.com</t>
+          <t>colaborador1@outlook.com</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>9495592907</v>
+        <v>9848299891</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -535,187 +535,1537 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>arquiteto de software</t>
+          <t>analista/desenvolvedor - alta plataforma</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>COLABORADOR 38</t>
+          <t>COLABORADOR 3</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>27652</v>
+        <v>24259</v>
       </c>
       <c r="C3" t="n">
-        <v>20625041130</v>
+        <v>48737508899</v>
       </c>
       <c r="D3" t="n">
-        <v>2132799</v>
+        <v>7949084</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ORG4</t>
+          <t>ORG1</t>
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>25065</v>
+        <v>30205</v>
       </c>
       <c r="G3" t="n">
-        <v>98142102444</v>
+        <v>45915006606</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>colaborador38@outlook.com</t>
+          <t>colaborador3@outlook.com</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>9795732223</v>
+        <v>9568300023</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>ABC - SP</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>arquiteto de software</t>
+          <t>analista/desenvolvedor - alta plataforma</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>COLABORADOR 43</t>
+          <t>COLABORADOR 5</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>35578</v>
+        <v>23033</v>
       </c>
       <c r="C4" t="n">
-        <v>74481389152</v>
+        <v>75327862923</v>
       </c>
       <c r="D4" t="n">
-        <v>3851831</v>
+        <v>1075350</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ORG1</t>
+          <t>ORG3</t>
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>23652</v>
+        <v>35711</v>
       </c>
       <c r="G4" t="n">
-        <v>55696242623</v>
+        <v>37668984314</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>colaborador43@outlook.com</t>
+          <t>colaborador5@outlook.com</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>9566498441</v>
+        <v>9670712796</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>DEF</t>
+          <t>ABC - SP</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>arquiteto de software</t>
+          <t>analista/desenvolvedor - alta plataforma</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>COLABORADOR 64</t>
+          <t>COLABORADOR 6</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>32599</v>
+        <v>24186</v>
       </c>
       <c r="C5" t="n">
-        <v>46528918935</v>
+        <v>85945316180</v>
       </c>
       <c r="D5" t="n">
-        <v>5442769</v>
+        <v>9795072</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ORG4</t>
+          <t>ORG1</t>
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>25841</v>
+        <v>28436</v>
       </c>
       <c r="G5" t="n">
-        <v>61232376686</v>
+        <v>44878846442</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>colaborador64@outlook.com</t>
+          <t>colaborador6@outlook.com</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>9399460190</v>
+        <v>9284449523</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>JKL</t>
+          <t>ABC - SP</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>arquiteto de software</t>
+          <t>analista/desenvolvedor - alta plataforma</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>COLABORADOR 65</t>
+          <t>COLABORADOR 11</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>30955</v>
+        <v>23295</v>
       </c>
       <c r="C6" t="n">
-        <v>14565609734</v>
+        <v>90954492477</v>
       </c>
       <c r="D6" t="n">
-        <v>1145907</v>
+        <v>4923680</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>ORG2</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>35241</v>
+      </c>
+      <c r="G6" t="n">
+        <v>17744105341</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>colaborador11@outlook.com</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>9373940977</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>ABC - SP</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>COLABORADOR 12</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>34715</v>
+      </c>
+      <c r="C7" t="n">
+        <v>79698532368</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3625745</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>36830</v>
+      </c>
+      <c r="G7" t="n">
+        <v>65531070330</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>colaborador12@outlook.com</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>9273870304</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>ABC - SP</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>COLABORADOR 14</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>32789</v>
+      </c>
+      <c r="C8" t="n">
+        <v>72563385852</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3288791</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ORG4</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>25844</v>
+      </c>
+      <c r="G8" t="n">
+        <v>11200265817</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>colaborador14@outlook.com</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>9604869326</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>ABC - SP</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>COLABORADOR 15</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>34147</v>
+      </c>
+      <c r="C9" t="n">
+        <v>40608279118</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6997153</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>ORG1</t>
         </is>
       </c>
-      <c r="F6" s="2" t="n">
-        <v>27098</v>
-      </c>
-      <c r="G6" t="n">
-        <v>27386045269</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>colaborador65@outlook.com</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>9375112432</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>JKL</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>arquiteto de software</t>
+      <c r="F9" s="2" t="n">
+        <v>34976</v>
+      </c>
+      <c r="G9" t="n">
+        <v>11410371595</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>colaborador15@outlook.com</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>9765046508</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>ABC - SP</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>COLABORADOR 17</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>33213</v>
+      </c>
+      <c r="C10" t="n">
+        <v>70271104816</v>
+      </c>
+      <c r="D10" t="n">
+        <v>9277015</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ORG1</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>27951</v>
+      </c>
+      <c r="G10" t="n">
+        <v>21552438139</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>colaborador17@outlook.com</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>9607176675</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>ABC - SP</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>COLABORADOR 18</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>26337</v>
+      </c>
+      <c r="C11" t="n">
+        <v>75637965313</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4362611</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ORG2</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>36639</v>
+      </c>
+      <c r="G11" t="n">
+        <v>45952700882</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>colaborador18@outlook.com</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>9779834457</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>ABC - SP</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>COLABORADOR 22</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>34007</v>
+      </c>
+      <c r="C12" t="n">
+        <v>30021719597</v>
+      </c>
+      <c r="D12" t="n">
+        <v>7851986</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>ORG2</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>36151</v>
+      </c>
+      <c r="G12" t="n">
+        <v>97256715341</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>colaborador22@outlook.com</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>9492431715</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>ABC - SP</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>COLABORADOR 23</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>29285</v>
+      </c>
+      <c r="C13" t="n">
+        <v>44488662153</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7703695</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ORG4</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>31783</v>
+      </c>
+      <c r="G13" t="n">
+        <v>71407390098</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>colaborador23@outlook.com</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>9150384997</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>ABC - SP</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>COLABORADOR 25</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>23927</v>
+      </c>
+      <c r="C14" t="n">
+        <v>60867910572</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2797847</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>ORG2</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>29500</v>
+      </c>
+      <c r="G14" t="n">
+        <v>90263704506</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>colaborador25@outlook.com</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>9572596352</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>COLABORADOR 26</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>28440</v>
+      </c>
+      <c r="C15" t="n">
+        <v>31079092204</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5014020</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>26924</v>
+      </c>
+      <c r="G15" t="n">
+        <v>19662789887</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>colaborador26@outlook.com</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>9808995196</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>COLABORADOR 28</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>29286</v>
+      </c>
+      <c r="C16" t="n">
+        <v>93377713265</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5912139</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ORG1</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>31377</v>
+      </c>
+      <c r="G16" t="n">
+        <v>33015001215</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>colaborador28@outlook.com</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>9910268471</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>COLABORADOR 31</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>25364</v>
+      </c>
+      <c r="C17" t="n">
+        <v>13917639772</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2275423</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>ORG4</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>34233</v>
+      </c>
+      <c r="G17" t="n">
+        <v>30002217906</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>colaborador31@outlook.com</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>9301681654</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>COLABORADOR 33</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>35983</v>
+      </c>
+      <c r="C18" t="n">
+        <v>92051821486</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1817343</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>36746</v>
+      </c>
+      <c r="G18" t="n">
+        <v>92875833716</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>colaborador33@outlook.com</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>9872582548</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>COLABORADOR 34</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>29005</v>
+      </c>
+      <c r="C19" t="n">
+        <v>98089663655</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2989924</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>ORG4</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>22109</v>
+      </c>
+      <c r="G19" t="n">
+        <v>15655895816</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>colaborador34@outlook.com</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>9775645189</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>COLABORADOR 35</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>22198</v>
+      </c>
+      <c r="C20" t="n">
+        <v>94886028716</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8370681</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>32420</v>
+      </c>
+      <c r="G20" t="n">
+        <v>75550721049</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>colaborador35@outlook.com</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>9948694343</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>COLABORADOR 41</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>27916</v>
+      </c>
+      <c r="C21" t="n">
+        <v>28303445953</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4897956</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>26634</v>
+      </c>
+      <c r="G21" t="n">
+        <v>57173111062</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>colaborador41@outlook.com</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>9283683292</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>COLABORADOR 42</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>35354</v>
+      </c>
+      <c r="C22" t="n">
+        <v>30637944062</v>
+      </c>
+      <c r="D22" t="n">
+        <v>9871872</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>ORG4</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>23857</v>
+      </c>
+      <c r="G22" t="n">
+        <v>56047243374</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>colaborador42@outlook.com</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>9379732090</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>COLABORADOR 45</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>29778</v>
+      </c>
+      <c r="C23" t="n">
+        <v>66480466049</v>
+      </c>
+      <c r="D23" t="n">
+        <v>6149684</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>27559</v>
+      </c>
+      <c r="G23" t="n">
+        <v>62987935864</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>colaborador45@outlook.com</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>9158943070</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>COLABORADOR 48</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>27248</v>
+      </c>
+      <c r="C24" t="n">
+        <v>69026407529</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2891464</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>ORG4</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>27659</v>
+      </c>
+      <c r="G24" t="n">
+        <v>15387107611</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>colaborador48@outlook.com</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>9701527960</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>COLABORADOR 49</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>24536</v>
+      </c>
+      <c r="C25" t="n">
+        <v>28312867507</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5965737</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>ORG4</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>23177</v>
+      </c>
+      <c r="G25" t="n">
+        <v>58157695482</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>colaborador49@outlook.com</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>9642781827</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>COLABORADOR 54</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>22049</v>
+      </c>
+      <c r="C26" t="n">
+        <v>78432147560</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1433458</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>33790</v>
+      </c>
+      <c r="G26" t="n">
+        <v>49581483902</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>colaborador54@outlook.com</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>9635656492</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>GHI</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>COLABORADOR 55</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>34177</v>
+      </c>
+      <c r="C27" t="n">
+        <v>57915665377</v>
+      </c>
+      <c r="D27" t="n">
+        <v>7521932</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>ORG2</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>33979</v>
+      </c>
+      <c r="G27" t="n">
+        <v>58554051144</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>colaborador55@outlook.com</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>9733202083</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>GHI</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>COLABORADOR 57</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>35085</v>
+      </c>
+      <c r="C28" t="n">
+        <v>90450590323</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1068463</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>32011</v>
+      </c>
+      <c r="G28" t="n">
+        <v>72670844811</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>colaborador57@outlook.com</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>9707862007</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>GHI</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>COLABORADOR 83</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>33185</v>
+      </c>
+      <c r="C29" t="n">
+        <v>56151392715</v>
+      </c>
+      <c r="D29" t="n">
+        <v>8239645</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>ORG4</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>34953</v>
+      </c>
+      <c r="G29" t="n">
+        <v>27598149773</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>colaborador83@outlook.com</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>9447963101</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>MNO - DF</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>COLABORADOR 84</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>35013</v>
+      </c>
+      <c r="C30" t="n">
+        <v>63384049551</v>
+      </c>
+      <c r="D30" t="n">
+        <v>8294960</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>ORG1</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>29398</v>
+      </c>
+      <c r="G30" t="n">
+        <v>24489713610</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>colaborador84@outlook.com</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>9532468595</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>MNO - DF</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>COLABORADOR 86</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>24471</v>
+      </c>
+      <c r="C31" t="n">
+        <v>39205218007</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1815188</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>22758</v>
+      </c>
+      <c r="G31" t="n">
+        <v>15864883636</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>colaborador86@outlook.com</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>9359879116</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>MNO - DF</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>COLABORADOR 87</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>28690</v>
+      </c>
+      <c r="C32" t="n">
+        <v>12316308270</v>
+      </c>
+      <c r="D32" t="n">
+        <v>5154395</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>34736</v>
+      </c>
+      <c r="G32" t="n">
+        <v>77150033528</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>colaborador87@outlook.com</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>9867940655</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>MNO - DF</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>COLABORADOR 88</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>32204</v>
+      </c>
+      <c r="C33" t="n">
+        <v>31893325269</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1925142</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>ORG4</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>29022</v>
+      </c>
+      <c r="G33" t="n">
+        <v>72938967123</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>colaborador88@outlook.com</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>9305785095</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>MNO - DF</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>COLABORADOR 91</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>31804</v>
+      </c>
+      <c r="C34" t="n">
+        <v>94332141836</v>
+      </c>
+      <c r="D34" t="n">
+        <v>6750439</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>ORG2</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>28120</v>
+      </c>
+      <c r="G34" t="n">
+        <v>82059380577</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>colaborador91@outlook.com</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>9298876525</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>MNO - DF</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>COLABORADOR 94</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>26845</v>
+      </c>
+      <c r="C35" t="n">
+        <v>32920517033</v>
+      </c>
+      <c r="D35" t="n">
+        <v>9664966</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>34909</v>
+      </c>
+      <c r="G35" t="n">
+        <v>38236923825</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>colaborador94@outlook.com</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>9955458566</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>MNO - DF</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>COLABORADOR 95</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>30378</v>
+      </c>
+      <c r="C36" t="n">
+        <v>15639674704</v>
+      </c>
+      <c r="D36" t="n">
+        <v>7887262</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>ORG3</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>27357</v>
+      </c>
+      <c r="G36" t="n">
+        <v>40407925162</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>colaborador95@outlook.com</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>9230316094</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>MNO - DF</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>analista/desenvolvedor - alta plataforma</t>
         </is>
       </c>
     </row>

</xml_diff>